<commit_message>
Relatório Projecto Final + schemas das noticias
</commit_message>
<xml_diff>
--- a/Relatório Projecto Final/Schemas/News/NewsSchema.xlsx
+++ b/Relatório Projecto Final/Schemas/News/NewsSchema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\ISEL\Repositorio Local\PDM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\ISEL\Repositorio Local\PDM\Relatório Projecto Final\Schemas\News\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>MainActivity</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>NewsItem []</t>
+  </si>
+  <si>
+    <t>NewsCustomAdapter</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,12 +231,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -245,10 +242,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -662,6 +668,144 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="6455019" y="1633904"/>
           <a:ext cx="278423" cy="205154"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>197826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="615462" y="2337288"/>
+          <a:ext cx="0" cy="593481"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593481</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="608135" y="2930769"/>
+          <a:ext cx="3780692" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3363058" y="981808"/>
+          <a:ext cx="1040423" cy="1743807"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -953,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,38 +1113,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
       <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="9"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
       <c r="H5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1008,10 +1152,10 @@
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H8" s="3"/>
@@ -1029,44 +1173,56 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="14" t="s">
+      <c r="B12" s="15"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="J12" s="14" t="s">
+      <c r="F12" s="8"/>
+      <c r="J12" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="5" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="A12:B12"/>

</xml_diff>

<commit_message>
adicionado ficheiro que contem modelo EA(Sheet 2). actualizado NewSchema.
</commit_message>
<xml_diff>
--- a/Relatório Projecto Final/Schemas/News/NewsSchema.xlsx
+++ b/Relatório Projecto Final/Schemas/News/NewsSchema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\ISEL\Repositorio Local\PDM\Relatório Projecto Final\Schemas\News\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lima\ISEL\Ano 3\Semestre 5\PDM\repositorio\Relatório Projecto Final\Schemas\News\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -242,13 +242,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -811,6 +811,54 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7327</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>7326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3795346" y="974481"/>
+          <a:ext cx="1831731" cy="1172307"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -1100,7 +1148,7 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,11 +1161,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="4"/>
@@ -1184,10 +1232,10 @@
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="D12" s="7"/>
       <c r="E12" s="12" t="s">
         <v>5</v>
@@ -1203,17 +1251,17 @@
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="15"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">

</xml_diff>